<commit_message>
New excel file that contains only valid data for testing.
</commit_message>
<xml_diff>
--- a/testdata/test_all_valid.xlsx
+++ b/testdata/test_all_valid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidrhp/rust/sconv/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F77DC4A-4AF0-604C-A08C-1B3701BB7FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5792D08-DA2E-9E42-AF94-A2490C622F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15580" xr2:uid="{FD191831-9341-BF45-805B-B88E93377763}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>four</t>
   </si>
@@ -75,6 +75,18 @@
   </si>
   <si>
     <t>column_9_date</t>
+  </si>
+  <si>
+    <t>column_5_boolean</t>
+  </si>
+  <si>
+    <t>column_6_boolean_as_string</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>TRUE</t>
   </si>
 </sst>
 </file>
@@ -438,22 +450,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD2D87D-74F5-2647-84F1-10232B1D266B}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -467,16 +482,22 @@
         <v>8</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -489,17 +510,23 @@
       <c r="D2" t="s">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="4">
+      <c r="I2" s="4">
         <v>45019</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>10</v>
       </c>
@@ -512,17 +539,24 @@
       <c r="D3" t="s">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="4">
+      <c r="I3" s="4">
         <v>45141</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>